<commit_message>
dcerpc pcap, updated results, test.rules
</commit_message>
<xml_diff>
--- a/test-results.xlsx
+++ b/test-results.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>pcap</t>
   </si>
@@ -148,6 +148,21 @@
   </si>
   <si>
     <t>http1.pcap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accept, host, method, uri, accept-enc, accept-lang, host-raw, request-header, request-line, uri-raw, user-agent, urilen, response-body, response-header, response-line, server, stat-code, stat-msg, content-len, content-type, header, header-raw, header-names, protocol, start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34, 35, 36, 37, 38, 39, 40, 43, 44, 45, 46, 47, 49, 50, 51, 52, 53, 54, 56, 57, 59, 60, 61, 62, 63</t>
+  </si>
+  <si>
+    <t>dcerpc.pcap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dcerpc - iface, opnum, stub-data</t>
+  </si>
+  <si>
+    <t>87,88,89</t>
   </si>
 </sst>
 </file>
@@ -209,17 +224,35 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -727,57 +760,57 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" min="1" max="1" width="27.7109375"/>
-    <col bestFit="1" customWidth="1" min="2" max="2" width="26.7109375"/>
-    <col customWidth="1" min="3" max="3" style="1" width="20.57421875"/>
-    <col customWidth="1" min="4" max="4" width="24.140625"/>
+    <col bestFit="1" customWidth="1" min="1" max="1" style="1" width="27.7109375"/>
+    <col bestFit="1" customWidth="1" min="2" max="2" style="2" width="26.7109375"/>
+    <col customWidth="1" min="3" max="3" style="2" width="20.57421875"/>
+    <col customWidth="1" min="4" max="4" style="2" width="24.140625"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" t="s">
+      <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="6">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="6">
         <v>3</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -785,201 +818,242 @@
       <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="6">
         <v>4</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5" t="s">
+      <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" t="s">
+      <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7" t="s">
+      <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="6">
         <v>13</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" ht="14.25">
-      <c r="A8" t="s">
+      <c r="A8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="6">
         <v>14</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9" t="s">
+      <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="6">
         <v>15</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" t="s">
+      <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="6">
         <v>16</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" t="s">
+      <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="6">
         <v>17</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" ht="14.25">
-      <c r="A12" t="s">
+      <c r="A12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="6">
         <v>18</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="13" ht="14.25">
-      <c r="A13" t="s">
+      <c r="A13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="14" ht="14.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="6">
         <v>23</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="15" ht="14.25">
-      <c r="A15" t="s">
+      <c r="A15" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" ht="14.25">
-      <c r="A16" s="4" t="s">
+      <c r="D15" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" ht="42.75">
+      <c r="A16" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="6">
         <v>32</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="6" t="s">
         <v>40</v>
       </c>
     </row>
+    <row r="17" ht="14.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+    </row>
     <row r="18" ht="14.25">
-      <c r="A18" t="s">
+      <c r="A18" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" ht="14.25">
-      <c r="A19" t="s">
+      <c r="D18" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" ht="142.5">
+      <c r="A19" s="5" t="s">
         <v>44</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" ht="28.5">
+      <c r="A22" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
closing out testing by protocol
</commit_message>
<xml_diff>
--- a/test-results.xlsx
+++ b/test-results.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>pcap</t>
   </si>
@@ -205,6 +205,15 @@
   </si>
   <si>
     <t>file.name</t>
+  </si>
+  <si>
+    <t>krb5.cap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">msg_type, cname, sname, err_code, weak_encryption, ticket_encryption</t>
+  </si>
+  <si>
+    <t>112-7</t>
   </si>
 </sst>
 </file>
@@ -825,7 +834,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1171,6 +1180,20 @@
         <v>6</v>
       </c>
     </row>
+    <row r="25" ht="42.75">
+      <c r="A25" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
udp and testing updates
</commit_message>
<xml_diff>
--- a/test-results.xlsx
+++ b/test-results.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>pcap</t>
   </si>
@@ -36,15 +36,6 @@
     <t>yes</t>
   </si>
   <si>
-    <t>ipopts-eol.pcap</t>
-  </si>
-  <si>
-    <t>ipopts:eol</t>
-  </si>
-  <si>
-    <t>unk</t>
-  </si>
-  <si>
     <t>ipopts-nop.pcap</t>
   </si>
   <si>
@@ -114,28 +105,34 @@
     <t>19-22</t>
   </si>
   <si>
-    <t>tcp-mss.pcap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tcp mss</t>
+    <t>tcp-mss-hdr.pcap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tcp mss, hdr</t>
+  </si>
+  <si>
+    <t>23-4</t>
+  </si>
+  <si>
+    <t>udp.pcap</t>
+  </si>
+  <si>
+    <t>hdr</t>
   </si>
   <si>
     <t>icmp.pcap</t>
   </si>
   <si>
-    <t xml:space="preserve">icmp type,code,id,seq</t>
-  </si>
-  <si>
-    <t>26-9</t>
+    <t xml:space="preserve">icmp type,code,id,seq,hdr</t>
+  </si>
+  <si>
+    <t>26-30</t>
   </si>
   <si>
     <t>icmpv6.pcap</t>
   </si>
   <si>
-    <t>icmpv6.mtu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">datalink type 229 not (yet) supported in module PcapFile.</t>
+    <t>icmpv6.hdr</t>
   </si>
   <si>
     <t>sshv2.pcap</t>
@@ -233,7 +230,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,12 +253,6 @@
       <patternFill patternType="solid">
         <fgColor indexed="5"/>
         <bgColor indexed="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="2"/>
-        <bgColor indexed="2"/>
       </patternFill>
     </fill>
   </fills>
@@ -292,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -312,16 +303,13 @@
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="1" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -834,7 +822,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -875,28 +863,28 @@
       </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" s="6">
-        <v>4</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>6</v>
@@ -909,7 +897,7 @@
       <c r="B5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="6" t="s">
@@ -923,8 +911,8 @@
       <c r="B6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>17</v>
+      <c r="C6" s="6">
+        <v>13</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>6</v>
@@ -932,13 +920,13 @@
     </row>
     <row r="7" ht="14.25">
       <c r="A7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="C7" s="6">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>6</v>
@@ -946,13 +934,13 @@
     </row>
     <row r="8" ht="14.25">
       <c r="A8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="C8" s="6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>6</v>
@@ -960,13 +948,13 @@
     </row>
     <row r="9" ht="14.25">
       <c r="A9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="C9" s="6">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>6</v>
@@ -974,13 +962,13 @@
     </row>
     <row r="10" ht="14.25">
       <c r="A10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>25</v>
-      </c>
       <c r="C10" s="6">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>6</v>
@@ -988,13 +976,13 @@
     </row>
     <row r="11" ht="14.25">
       <c r="A11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>27</v>
-      </c>
       <c r="C11" s="6">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>6</v>
@@ -1002,26 +990,26 @@
     </row>
     <row r="12" ht="14.25">
       <c r="A12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="C12" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="6">
-        <v>18</v>
-      </c>
       <c r="D12" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="13" ht="14.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D13" s="6" t="s">
@@ -1029,27 +1017,27 @@
       </c>
     </row>
     <row r="14" ht="14.25">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="6">
-        <v>23</v>
-      </c>
-      <c r="D14" s="6" t="s">
+      <c r="C14" s="7">
+        <v>25</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="15" ht="14.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="7" t="s">
         <v>37</v>
       </c>
       <c r="D15" s="6" t="s">
@@ -1057,140 +1045,138 @@
       </c>
     </row>
     <row r="16" ht="42.75">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C16" s="6">
         <v>32</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" ht="42.75">
+      <c r="A17" s="8" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="17" ht="42.75">
-      <c r="A17" s="10" t="s">
+      <c r="B17" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="18" ht="14.25">
       <c r="A18" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="D18" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" ht="142.5">
+      <c r="A19" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" ht="142.5">
-      <c r="A19" s="7" t="s">
+      <c r="B19" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="C19" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="D19" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" ht="28.5">
+      <c r="A20" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" ht="28.5">
-      <c r="A20" s="10" t="s">
+      <c r="B20" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="D20" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="A21" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" ht="14.25">
-      <c r="A21" s="11" t="s">
+      <c r="B21" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="C21" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>55</v>
       </c>
       <c r="D21" s="6"/>
     </row>
     <row r="22" ht="28.5">
       <c r="A22" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="C22" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="D22" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" ht="28.5">
+      <c r="A23" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" ht="28.5">
-      <c r="A23" s="10" t="s">
+      <c r="B23" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="D23" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="A24" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" ht="14.25">
-      <c r="A24" s="10" t="s">
+      <c r="B24" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>63</v>
       </c>
       <c r="C24" s="6">
         <v>102</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="25" ht="42.75">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="7" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>